<commit_message>
changed DC power jack in BOM
metal jack body + center negative  = ground short
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chris/Documents/GitHub/buffer-pedal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1FFFFE07-9121-1749-8747-B8935157A8C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7EB63AAB-5EC1-3B4B-B80E-2971BD4F5886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{07A1FDCE-47C8-3949-82B4-30B89939407E}"/>
+    <workbookView xWindow="1300" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{07A1FDCE-47C8-3949-82B4-30B89939407E}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,6 @@
     <t xml:space="preserve"> 859-LTL2R3KGD-EM</t>
   </si>
   <si>
-    <t xml:space="preserve"> 163-R123B-E</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 568-NYS229</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>DC Power Connector</t>
+  </si>
+  <si>
+    <t>163-1060-EX</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -607,7 +607,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
         <v>36</v>
@@ -627,7 +627,7 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
@@ -647,7 +647,7 @@
         <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
         <v>33</v>
@@ -667,7 +667,7 @@
         <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
         <v>40</v>
@@ -727,7 +727,7 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
@@ -761,13 +761,13 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -778,13 +778,13 @@
         <v>31</v>
       </c>
       <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
         <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>